<commit_message>
Adding a condition pattern
計算条件の追加
</commit_message>
<xml_diff>
--- a/test/schedule.xlsx
+++ b/test/schedule.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="schedule" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="schedule2" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
   <si>
     <t xml:space="preserve">parameter</t>
   </si>
@@ -126,9 +127,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -334,7 +336,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -455,13 +457,12 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="D4:E4 B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.12890625" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="10.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -521,15 +522,13 @@
   </sheetPr>
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F9" activeCellId="1" sqref="D4:E4 F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.12890625" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="10.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="11.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="10.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1432,4 +1431,888 @@
     <oddFooter>&amp;C&amp;"Times New Roman,標準"&amp;12ページ &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:N18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4:E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.12890625" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="11.86"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="C2" s="7" t="n">
+        <f aca="false">IF($B2&lt;&gt;"",AND($D2&lt;&gt;"",$E2&lt;&gt;""),"")</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="10" t="n">
+        <f aca="false">IF($D2="","",IF(AND(TIMEVALUE(F$1)&gt;=TIMEVALUE($D2),TIMEVALUE(F$1)&lt;TIMEVALUE($E2)),1,""))</f>
+        <v>1</v>
+      </c>
+      <c r="G2" s="10" t="n">
+        <f aca="false">IF($D2="","",IF(AND(TIMEVALUE(G$1)&gt;=TIMEVALUE($D2),TIMEVALUE(G$1)&lt;TIMEVALUE($E2)),1,""))</f>
+        <v>1</v>
+      </c>
+      <c r="H2" s="10" t="str">
+        <f aca="false">IF($D2="","",IF(AND(TIMEVALUE(H$1)&gt;=TIMEVALUE($D2),TIMEVALUE(H$1)&lt;TIMEVALUE($E2)),1,""))</f>
+        <v/>
+      </c>
+      <c r="I2" s="10" t="str">
+        <f aca="false">IF($D2="","",IF(AND(TIMEVALUE(I$1)&gt;=TIMEVALUE($D2),TIMEVALUE(I$1)&lt;TIMEVALUE($E2)),1,""))</f>
+        <v/>
+      </c>
+      <c r="J2" s="10" t="str">
+        <f aca="false">IF($D2="","",IF(AND(TIMEVALUE(J$1)&gt;=TIMEVALUE($D2),TIMEVALUE(J$1)&lt;TIMEVALUE($E2)),1,""))</f>
+        <v/>
+      </c>
+      <c r="K2" s="10" t="str">
+        <f aca="false">IF($D2="","",IF(AND(TIMEVALUE(K$1)&gt;=TIMEVALUE($D2),TIMEVALUE(K$1)&lt;TIMEVALUE($E2)),1,""))</f>
+        <v/>
+      </c>
+      <c r="L2" s="10" t="str">
+        <f aca="false">IF($D2="","",IF(AND(TIMEVALUE(L$1)&gt;=TIMEVALUE($D2),TIMEVALUE(L$1)&lt;TIMEVALUE($E2)),1,""))</f>
+        <v/>
+      </c>
+      <c r="M2" s="10" t="str">
+        <f aca="false">IF($D2="","",IF(AND(TIMEVALUE(M$1)&gt;=TIMEVALUE($D2),TIMEVALUE(M$1)&lt;TIMEVALUE($E2)),1,""))</f>
+        <v/>
+      </c>
+      <c r="N2" s="10" t="str">
+        <f aca="false">IF($D2="","",IF(AND(TIMEVALUE(N$1)&gt;=TIMEVALUE($D2),TIMEVALUE(N$1)&lt;TIMEVALUE($E2)),1,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="11" t="n">
+        <v>30</v>
+      </c>
+      <c r="C3" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="10" t="str">
+        <f aca="false">IF($D3="","",IF(AND(TIMEVALUE(F$1)&gt;=TIMEVALUE($D3),TIMEVALUE(F$1)&lt;TIMEVALUE($E3)),1,""))</f>
+        <v/>
+      </c>
+      <c r="G3" s="10" t="n">
+        <f aca="false">IF($D3="","",IF(AND(TIMEVALUE(G$1)&gt;=TIMEVALUE($D3),TIMEVALUE(G$1)&lt;TIMEVALUE($E3)),1,""))</f>
+        <v>1</v>
+      </c>
+      <c r="H3" s="10" t="n">
+        <f aca="false">IF($D3="","",IF(AND(TIMEVALUE(H$1)&gt;=TIMEVALUE($D3),TIMEVALUE(H$1)&lt;TIMEVALUE($E3)),1,""))</f>
+        <v>1</v>
+      </c>
+      <c r="I3" s="10" t="n">
+        <f aca="false">IF($D3="","",IF(AND(TIMEVALUE(I$1)&gt;=TIMEVALUE($D3),TIMEVALUE(I$1)&lt;TIMEVALUE($E3)),1,""))</f>
+        <v>1</v>
+      </c>
+      <c r="J3" s="10" t="n">
+        <f aca="false">IF($D3="","",IF(AND(TIMEVALUE(J$1)&gt;=TIMEVALUE($D3),TIMEVALUE(J$1)&lt;TIMEVALUE($E3)),1,""))</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="10" t="n">
+        <f aca="false">IF($D3="","",IF(AND(TIMEVALUE(K$1)&gt;=TIMEVALUE($D3),TIMEVALUE(K$1)&lt;TIMEVALUE($E3)),1,""))</f>
+        <v>1</v>
+      </c>
+      <c r="L3" s="10" t="n">
+        <f aca="false">IF($D3="","",IF(AND(TIMEVALUE(L$1)&gt;=TIMEVALUE($D3),TIMEVALUE(L$1)&lt;TIMEVALUE($E3)),1,""))</f>
+        <v>1</v>
+      </c>
+      <c r="M3" s="10" t="str">
+        <f aca="false">IF($D3="","",IF(AND(TIMEVALUE(M$1)&gt;=TIMEVALUE($D3),TIMEVALUE(M$1)&lt;TIMEVALUE($E3)),1,""))</f>
+        <v/>
+      </c>
+      <c r="N3" s="10" t="str">
+        <f aca="false">IF($D3="","",IF(AND(TIMEVALUE(N$1)&gt;=TIMEVALUE($D3),TIMEVALUE(N$1)&lt;TIMEVALUE($E3)),1,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="11" t="n">
+        <v>30</v>
+      </c>
+      <c r="C4" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="10" t="str">
+        <f aca="false">IF($D4="","",IF(AND(TIMEVALUE(F$1)&gt;=TIMEVALUE($D4),TIMEVALUE(F$1)&lt;TIMEVALUE($E4)),1,""))</f>
+        <v/>
+      </c>
+      <c r="G4" s="10" t="n">
+        <f aca="false">IF($D4="","",IF(AND(TIMEVALUE(G$1)&gt;=TIMEVALUE($D4),TIMEVALUE(G$1)&lt;TIMEVALUE($E4)),1,""))</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="10" t="n">
+        <f aca="false">IF($D4="","",IF(AND(TIMEVALUE(H$1)&gt;=TIMEVALUE($D4),TIMEVALUE(H$1)&lt;TIMEVALUE($E4)),1,""))</f>
+        <v>1</v>
+      </c>
+      <c r="I4" s="10" t="n">
+        <f aca="false">IF($D4="","",IF(AND(TIMEVALUE(I$1)&gt;=TIMEVALUE($D4),TIMEVALUE(I$1)&lt;TIMEVALUE($E4)),1,""))</f>
+        <v>1</v>
+      </c>
+      <c r="J4" s="10" t="n">
+        <f aca="false">IF($D4="","",IF(AND(TIMEVALUE(J$1)&gt;=TIMEVALUE($D4),TIMEVALUE(J$1)&lt;TIMEVALUE($E4)),1,""))</f>
+        <v>1</v>
+      </c>
+      <c r="K4" s="10" t="n">
+        <f aca="false">IF($D4="","",IF(AND(TIMEVALUE(K$1)&gt;=TIMEVALUE($D4),TIMEVALUE(K$1)&lt;TIMEVALUE($E4)),1,""))</f>
+        <v>1</v>
+      </c>
+      <c r="L4" s="10" t="n">
+        <f aca="false">IF($D4="","",IF(AND(TIMEVALUE(L$1)&gt;=TIMEVALUE($D4),TIMEVALUE(L$1)&lt;TIMEVALUE($E4)),1,""))</f>
+        <v>1</v>
+      </c>
+      <c r="M4" s="10" t="str">
+        <f aca="false">IF($D4="","",IF(AND(TIMEVALUE(M$1)&gt;=TIMEVALUE($D4),TIMEVALUE(M$1)&lt;TIMEVALUE($E4)),1,""))</f>
+        <v/>
+      </c>
+      <c r="N4" s="10" t="str">
+        <f aca="false">IF($D4="","",IF(AND(TIMEVALUE(N$1)&gt;=TIMEVALUE($D4),TIMEVALUE(N$1)&lt;TIMEVALUE($E4)),1,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="11" t="n">
+        <v>30</v>
+      </c>
+      <c r="C5" s="11" t="n">
+        <f aca="false">IF($B5&lt;&gt;"",AND($D5&lt;&gt;"",$E5&lt;&gt;""),"")</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="10" t="str">
+        <f aca="false">IF($D5="","",IF(AND(TIMEVALUE(F$1)&gt;=TIMEVALUE($D5),TIMEVALUE(F$1)&lt;TIMEVALUE($E5)),1,""))</f>
+        <v/>
+      </c>
+      <c r="G5" s="10" t="str">
+        <f aca="false">IF($D5="","",IF(AND(TIMEVALUE(G$1)&gt;=TIMEVALUE($D5),TIMEVALUE(G$1)&lt;TIMEVALUE($E5)),1,""))</f>
+        <v/>
+      </c>
+      <c r="H5" s="10" t="str">
+        <f aca="false">IF($D5="","",IF(AND(TIMEVALUE(H$1)&gt;=TIMEVALUE($D5),TIMEVALUE(H$1)&lt;TIMEVALUE($E5)),1,""))</f>
+        <v/>
+      </c>
+      <c r="I5" s="10" t="str">
+        <f aca="false">IF($D5="","",IF(AND(TIMEVALUE(I$1)&gt;=TIMEVALUE($D5),TIMEVALUE(I$1)&lt;TIMEVALUE($E5)),1,""))</f>
+        <v/>
+      </c>
+      <c r="J5" s="10" t="str">
+        <f aca="false">IF($D5="","",IF(AND(TIMEVALUE(J$1)&gt;=TIMEVALUE($D5),TIMEVALUE(J$1)&lt;TIMEVALUE($E5)),1,""))</f>
+        <v/>
+      </c>
+      <c r="K5" s="10" t="str">
+        <f aca="false">IF($D5="","",IF(AND(TIMEVALUE(K$1)&gt;=TIMEVALUE($D5),TIMEVALUE(K$1)&lt;TIMEVALUE($E5)),1,""))</f>
+        <v/>
+      </c>
+      <c r="L5" s="10" t="str">
+        <f aca="false">IF($D5="","",IF(AND(TIMEVALUE(L$1)&gt;=TIMEVALUE($D5),TIMEVALUE(L$1)&lt;TIMEVALUE($E5)),1,""))</f>
+        <v/>
+      </c>
+      <c r="M5" s="10" t="str">
+        <f aca="false">IF($D5="","",IF(AND(TIMEVALUE(M$1)&gt;=TIMEVALUE($D5),TIMEVALUE(M$1)&lt;TIMEVALUE($E5)),1,""))</f>
+        <v/>
+      </c>
+      <c r="N5" s="10" t="str">
+        <f aca="false">IF($D5="","",IF(AND(TIMEVALUE(N$1)&gt;=TIMEVALUE($D5),TIMEVALUE(N$1)&lt;TIMEVALUE($E5)),1,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11" t="str">
+        <f aca="false">IF($B6&lt;&gt;"",AND($D6&lt;&gt;"",$E6&lt;&gt;""),"")</f>
+        <v/>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="10" t="str">
+        <f aca="false">IF($D6="","",IF(AND(TIMEVALUE(F$1)&gt;=TIMEVALUE($D6),TIMEVALUE(F$1)&lt;TIMEVALUE($E6)),1,""))</f>
+        <v/>
+      </c>
+      <c r="G6" s="10" t="str">
+        <f aca="false">IF($D6="","",IF(AND(TIMEVALUE(G$1)&gt;=TIMEVALUE($D6),TIMEVALUE(G$1)&lt;TIMEVALUE($E6)),1,""))</f>
+        <v/>
+      </c>
+      <c r="H6" s="10" t="str">
+        <f aca="false">IF($D6="","",IF(AND(TIMEVALUE(H$1)&gt;=TIMEVALUE($D6),TIMEVALUE(H$1)&lt;TIMEVALUE($E6)),1,""))</f>
+        <v/>
+      </c>
+      <c r="I6" s="10" t="str">
+        <f aca="false">IF($D6="","",IF(AND(TIMEVALUE(I$1)&gt;=TIMEVALUE($D6),TIMEVALUE(I$1)&lt;TIMEVALUE($E6)),1,""))</f>
+        <v/>
+      </c>
+      <c r="J6" s="10" t="str">
+        <f aca="false">IF($D6="","",IF(AND(TIMEVALUE(J$1)&gt;=TIMEVALUE($D6),TIMEVALUE(J$1)&lt;TIMEVALUE($E6)),1,""))</f>
+        <v/>
+      </c>
+      <c r="K6" s="10" t="str">
+        <f aca="false">IF($D6="","",IF(AND(TIMEVALUE(K$1)&gt;=TIMEVALUE($D6),TIMEVALUE(K$1)&lt;TIMEVALUE($E6)),1,""))</f>
+        <v/>
+      </c>
+      <c r="L6" s="10" t="str">
+        <f aca="false">IF($D6="","",IF(AND(TIMEVALUE(L$1)&gt;=TIMEVALUE($D6),TIMEVALUE(L$1)&lt;TIMEVALUE($E6)),1,""))</f>
+        <v/>
+      </c>
+      <c r="M6" s="10" t="str">
+        <f aca="false">IF($D6="","",IF(AND(TIMEVALUE(M$1)&gt;=TIMEVALUE($D6),TIMEVALUE(M$1)&lt;TIMEVALUE($E6)),1,""))</f>
+        <v/>
+      </c>
+      <c r="N6" s="10" t="str">
+        <f aca="false">IF($D6="","",IF(AND(TIMEVALUE(N$1)&gt;=TIMEVALUE($D6),TIMEVALUE(N$1)&lt;TIMEVALUE($E6)),1,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11" t="str">
+        <f aca="false">IF($B7&lt;&gt;"",AND($D7&lt;&gt;"",$E7&lt;&gt;""),"")</f>
+        <v/>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="10" t="str">
+        <f aca="false">IF($D7="","",IF(AND(TIMEVALUE(F$1)&gt;=TIMEVALUE($D7),TIMEVALUE(F$1)&lt;TIMEVALUE($E7)),1,""))</f>
+        <v/>
+      </c>
+      <c r="G7" s="10" t="str">
+        <f aca="false">IF($D7="","",IF(AND(TIMEVALUE(G$1)&gt;=TIMEVALUE($D7),TIMEVALUE(G$1)&lt;TIMEVALUE($E7)),1,""))</f>
+        <v/>
+      </c>
+      <c r="H7" s="10" t="str">
+        <f aca="false">IF($D7="","",IF(AND(TIMEVALUE(H$1)&gt;=TIMEVALUE($D7),TIMEVALUE(H$1)&lt;TIMEVALUE($E7)),1,""))</f>
+        <v/>
+      </c>
+      <c r="I7" s="10" t="str">
+        <f aca="false">IF($D7="","",IF(AND(TIMEVALUE(I$1)&gt;=TIMEVALUE($D7),TIMEVALUE(I$1)&lt;TIMEVALUE($E7)),1,""))</f>
+        <v/>
+      </c>
+      <c r="J7" s="10" t="str">
+        <f aca="false">IF($D7="","",IF(AND(TIMEVALUE(J$1)&gt;=TIMEVALUE($D7),TIMEVALUE(J$1)&lt;TIMEVALUE($E7)),1,""))</f>
+        <v/>
+      </c>
+      <c r="K7" s="10" t="str">
+        <f aca="false">IF($D7="","",IF(AND(TIMEVALUE(K$1)&gt;=TIMEVALUE($D7),TIMEVALUE(K$1)&lt;TIMEVALUE($E7)),1,""))</f>
+        <v/>
+      </c>
+      <c r="L7" s="10" t="str">
+        <f aca="false">IF($D7="","",IF(AND(TIMEVALUE(L$1)&gt;=TIMEVALUE($D7),TIMEVALUE(L$1)&lt;TIMEVALUE($E7)),1,""))</f>
+        <v/>
+      </c>
+      <c r="M7" s="10" t="str">
+        <f aca="false">IF($D7="","",IF(AND(TIMEVALUE(M$1)&gt;=TIMEVALUE($D7),TIMEVALUE(M$1)&lt;TIMEVALUE($E7)),1,""))</f>
+        <v/>
+      </c>
+      <c r="N7" s="10" t="str">
+        <f aca="false">IF($D7="","",IF(AND(TIMEVALUE(N$1)&gt;=TIMEVALUE($D7),TIMEVALUE(N$1)&lt;TIMEVALUE($E7)),1,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11" t="str">
+        <f aca="false">IF($B8&lt;&gt;"",AND($D8&lt;&gt;"",$E8&lt;&gt;""),"")</f>
+        <v/>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="10" t="str">
+        <f aca="false">IF($D8="","",IF(AND(TIMEVALUE(F$1)&gt;=TIMEVALUE($D8),TIMEVALUE(F$1)&lt;TIMEVALUE($E8)),1,""))</f>
+        <v/>
+      </c>
+      <c r="G8" s="10" t="str">
+        <f aca="false">IF($D8="","",IF(AND(TIMEVALUE(G$1)&gt;=TIMEVALUE($D8),TIMEVALUE(G$1)&lt;TIMEVALUE($E8)),1,""))</f>
+        <v/>
+      </c>
+      <c r="H8" s="10" t="str">
+        <f aca="false">IF($D8="","",IF(AND(TIMEVALUE(H$1)&gt;=TIMEVALUE($D8),TIMEVALUE(H$1)&lt;TIMEVALUE($E8)),1,""))</f>
+        <v/>
+      </c>
+      <c r="I8" s="10" t="str">
+        <f aca="false">IF($D8="","",IF(AND(TIMEVALUE(I$1)&gt;=TIMEVALUE($D8),TIMEVALUE(I$1)&lt;TIMEVALUE($E8)),1,""))</f>
+        <v/>
+      </c>
+      <c r="J8" s="10" t="str">
+        <f aca="false">IF($D8="","",IF(AND(TIMEVALUE(J$1)&gt;=TIMEVALUE($D8),TIMEVALUE(J$1)&lt;TIMEVALUE($E8)),1,""))</f>
+        <v/>
+      </c>
+      <c r="K8" s="10" t="str">
+        <f aca="false">IF($D8="","",IF(AND(TIMEVALUE(K$1)&gt;=TIMEVALUE($D8),TIMEVALUE(K$1)&lt;TIMEVALUE($E8)),1,""))</f>
+        <v/>
+      </c>
+      <c r="L8" s="10" t="str">
+        <f aca="false">IF($D8="","",IF(AND(TIMEVALUE(L$1)&gt;=TIMEVALUE($D8),TIMEVALUE(L$1)&lt;TIMEVALUE($E8)),1,""))</f>
+        <v/>
+      </c>
+      <c r="M8" s="10" t="str">
+        <f aca="false">IF($D8="","",IF(AND(TIMEVALUE(M$1)&gt;=TIMEVALUE($D8),TIMEVALUE(M$1)&lt;TIMEVALUE($E8)),1,""))</f>
+        <v/>
+      </c>
+      <c r="N8" s="10" t="str">
+        <f aca="false">IF($D8="","",IF(AND(TIMEVALUE(N$1)&gt;=TIMEVALUE($D8),TIMEVALUE(N$1)&lt;TIMEVALUE($E8)),1,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11" t="str">
+        <f aca="false">IF($B9&lt;&gt;"",AND($D9&lt;&gt;"",$E9&lt;&gt;""),"")</f>
+        <v/>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="10" t="str">
+        <f aca="false">IF($D9="","",IF(AND(TIMEVALUE(F$1)&gt;=TIMEVALUE($D9),TIMEVALUE(F$1)&lt;TIMEVALUE($E9)),1,""))</f>
+        <v/>
+      </c>
+      <c r="G9" s="10" t="str">
+        <f aca="false">IF($D9="","",IF(AND(TIMEVALUE(G$1)&gt;=TIMEVALUE($D9),TIMEVALUE(G$1)&lt;TIMEVALUE($E9)),1,""))</f>
+        <v/>
+      </c>
+      <c r="H9" s="10" t="str">
+        <f aca="false">IF($D9="","",IF(AND(TIMEVALUE(H$1)&gt;=TIMEVALUE($D9),TIMEVALUE(H$1)&lt;TIMEVALUE($E9)),1,""))</f>
+        <v/>
+      </c>
+      <c r="I9" s="10" t="str">
+        <f aca="false">IF($D9="","",IF(AND(TIMEVALUE(I$1)&gt;=TIMEVALUE($D9),TIMEVALUE(I$1)&lt;TIMEVALUE($E9)),1,""))</f>
+        <v/>
+      </c>
+      <c r="J9" s="10" t="str">
+        <f aca="false">IF($D9="","",IF(AND(TIMEVALUE(J$1)&gt;=TIMEVALUE($D9),TIMEVALUE(J$1)&lt;TIMEVALUE($E9)),1,""))</f>
+        <v/>
+      </c>
+      <c r="K9" s="10" t="str">
+        <f aca="false">IF($D9="","",IF(AND(TIMEVALUE(K$1)&gt;=TIMEVALUE($D9),TIMEVALUE(K$1)&lt;TIMEVALUE($E9)),1,""))</f>
+        <v/>
+      </c>
+      <c r="L9" s="10" t="str">
+        <f aca="false">IF($D9="","",IF(AND(TIMEVALUE(L$1)&gt;=TIMEVALUE($D9),TIMEVALUE(L$1)&lt;TIMEVALUE($E9)),1,""))</f>
+        <v/>
+      </c>
+      <c r="M9" s="10" t="str">
+        <f aca="false">IF($D9="","",IF(AND(TIMEVALUE(M$1)&gt;=TIMEVALUE($D9),TIMEVALUE(M$1)&lt;TIMEVALUE($E9)),1,""))</f>
+        <v/>
+      </c>
+      <c r="N9" s="10" t="str">
+        <f aca="false">IF($D9="","",IF(AND(TIMEVALUE(N$1)&gt;=TIMEVALUE($D9),TIMEVALUE(N$1)&lt;TIMEVALUE($E9)),1,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11" t="str">
+        <f aca="false">IF($B10&lt;&gt;"",AND($D10&lt;&gt;"",$E10&lt;&gt;""),"")</f>
+        <v/>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="10" t="str">
+        <f aca="false">IF($D10="","",IF(AND(TIMEVALUE(F$1)&gt;=TIMEVALUE($D10),TIMEVALUE(F$1)&lt;TIMEVALUE($E10)),1,""))</f>
+        <v/>
+      </c>
+      <c r="G10" s="10" t="str">
+        <f aca="false">IF($D10="","",IF(AND(TIMEVALUE(G$1)&gt;=TIMEVALUE($D10),TIMEVALUE(G$1)&lt;TIMEVALUE($E10)),1,""))</f>
+        <v/>
+      </c>
+      <c r="H10" s="10" t="str">
+        <f aca="false">IF($D10="","",IF(AND(TIMEVALUE(H$1)&gt;=TIMEVALUE($D10),TIMEVALUE(H$1)&lt;TIMEVALUE($E10)),1,""))</f>
+        <v/>
+      </c>
+      <c r="I10" s="10" t="str">
+        <f aca="false">IF($D10="","",IF(AND(TIMEVALUE(I$1)&gt;=TIMEVALUE($D10),TIMEVALUE(I$1)&lt;TIMEVALUE($E10)),1,""))</f>
+        <v/>
+      </c>
+      <c r="J10" s="10" t="str">
+        <f aca="false">IF($D10="","",IF(AND(TIMEVALUE(J$1)&gt;=TIMEVALUE($D10),TIMEVALUE(J$1)&lt;TIMEVALUE($E10)),1,""))</f>
+        <v/>
+      </c>
+      <c r="K10" s="10" t="str">
+        <f aca="false">IF($D10="","",IF(AND(TIMEVALUE(K$1)&gt;=TIMEVALUE($D10),TIMEVALUE(K$1)&lt;TIMEVALUE($E10)),1,""))</f>
+        <v/>
+      </c>
+      <c r="L10" s="10" t="str">
+        <f aca="false">IF($D10="","",IF(AND(TIMEVALUE(L$1)&gt;=TIMEVALUE($D10),TIMEVALUE(L$1)&lt;TIMEVALUE($E10)),1,""))</f>
+        <v/>
+      </c>
+      <c r="M10" s="10" t="str">
+        <f aca="false">IF($D10="","",IF(AND(TIMEVALUE(M$1)&gt;=TIMEVALUE($D10),TIMEVALUE(M$1)&lt;TIMEVALUE($E10)),1,""))</f>
+        <v/>
+      </c>
+      <c r="N10" s="10" t="str">
+        <f aca="false">IF($D10="","",IF(AND(TIMEVALUE(N$1)&gt;=TIMEVALUE($D10),TIMEVALUE(N$1)&lt;TIMEVALUE($E10)),1,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11" t="str">
+        <f aca="false">IF($B11&lt;&gt;"",AND($D11&lt;&gt;"",$E11&lt;&gt;""),"")</f>
+        <v/>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="10" t="str">
+        <f aca="false">IF($D11="","",IF(AND(TIMEVALUE(F$1)&gt;=TIMEVALUE($D11),TIMEVALUE(F$1)&lt;TIMEVALUE($E11)),1,""))</f>
+        <v/>
+      </c>
+      <c r="G11" s="10" t="str">
+        <f aca="false">IF($D11="","",IF(AND(TIMEVALUE(G$1)&gt;=TIMEVALUE($D11),TIMEVALUE(G$1)&lt;TIMEVALUE($E11)),1,""))</f>
+        <v/>
+      </c>
+      <c r="H11" s="10" t="str">
+        <f aca="false">IF($D11="","",IF(AND(TIMEVALUE(H$1)&gt;=TIMEVALUE($D11),TIMEVALUE(H$1)&lt;TIMEVALUE($E11)),1,""))</f>
+        <v/>
+      </c>
+      <c r="I11" s="10" t="str">
+        <f aca="false">IF($D11="","",IF(AND(TIMEVALUE(I$1)&gt;=TIMEVALUE($D11),TIMEVALUE(I$1)&lt;TIMEVALUE($E11)),1,""))</f>
+        <v/>
+      </c>
+      <c r="J11" s="10" t="str">
+        <f aca="false">IF($D11="","",IF(AND(TIMEVALUE(J$1)&gt;=TIMEVALUE($D11),TIMEVALUE(J$1)&lt;TIMEVALUE($E11)),1,""))</f>
+        <v/>
+      </c>
+      <c r="K11" s="10" t="str">
+        <f aca="false">IF($D11="","",IF(AND(TIMEVALUE(K$1)&gt;=TIMEVALUE($D11),TIMEVALUE(K$1)&lt;TIMEVALUE($E11)),1,""))</f>
+        <v/>
+      </c>
+      <c r="L11" s="10" t="str">
+        <f aca="false">IF($D11="","",IF(AND(TIMEVALUE(L$1)&gt;=TIMEVALUE($D11),TIMEVALUE(L$1)&lt;TIMEVALUE($E11)),1,""))</f>
+        <v/>
+      </c>
+      <c r="M11" s="10" t="str">
+        <f aca="false">IF($D11="","",IF(AND(TIMEVALUE(M$1)&gt;=TIMEVALUE($D11),TIMEVALUE(M$1)&lt;TIMEVALUE($E11)),1,""))</f>
+        <v/>
+      </c>
+      <c r="N11" s="10" t="str">
+        <f aca="false">IF($D11="","",IF(AND(TIMEVALUE(N$1)&gt;=TIMEVALUE($D11),TIMEVALUE(N$1)&lt;TIMEVALUE($E11)),1,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11" t="str">
+        <f aca="false">IF($B12&lt;&gt;"",AND($D12&lt;&gt;"",$E12&lt;&gt;""),"")</f>
+        <v/>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="10" t="str">
+        <f aca="false">IF($D12="","",IF(AND(TIMEVALUE(F$1)&gt;=TIMEVALUE($D12),TIMEVALUE(F$1)&lt;TIMEVALUE($E12)),1,""))</f>
+        <v/>
+      </c>
+      <c r="G12" s="10" t="str">
+        <f aca="false">IF($D12="","",IF(AND(TIMEVALUE(G$1)&gt;=TIMEVALUE($D12),TIMEVALUE(G$1)&lt;TIMEVALUE($E12)),1,""))</f>
+        <v/>
+      </c>
+      <c r="H12" s="10" t="str">
+        <f aca="false">IF($D12="","",IF(AND(TIMEVALUE(H$1)&gt;=TIMEVALUE($D12),TIMEVALUE(H$1)&lt;TIMEVALUE($E12)),1,""))</f>
+        <v/>
+      </c>
+      <c r="I12" s="10" t="str">
+        <f aca="false">IF($D12="","",IF(AND(TIMEVALUE(I$1)&gt;=TIMEVALUE($D12),TIMEVALUE(I$1)&lt;TIMEVALUE($E12)),1,""))</f>
+        <v/>
+      </c>
+      <c r="J12" s="10" t="str">
+        <f aca="false">IF($D12="","",IF(AND(TIMEVALUE(J$1)&gt;=TIMEVALUE($D12),TIMEVALUE(J$1)&lt;TIMEVALUE($E12)),1,""))</f>
+        <v/>
+      </c>
+      <c r="K12" s="10" t="str">
+        <f aca="false">IF($D12="","",IF(AND(TIMEVALUE(K$1)&gt;=TIMEVALUE($D12),TIMEVALUE(K$1)&lt;TIMEVALUE($E12)),1,""))</f>
+        <v/>
+      </c>
+      <c r="L12" s="10" t="str">
+        <f aca="false">IF($D12="","",IF(AND(TIMEVALUE(L$1)&gt;=TIMEVALUE($D12),TIMEVALUE(L$1)&lt;TIMEVALUE($E12)),1,""))</f>
+        <v/>
+      </c>
+      <c r="M12" s="10" t="str">
+        <f aca="false">IF($D12="","",IF(AND(TIMEVALUE(M$1)&gt;=TIMEVALUE($D12),TIMEVALUE(M$1)&lt;TIMEVALUE($E12)),1,""))</f>
+        <v/>
+      </c>
+      <c r="N12" s="10" t="str">
+        <f aca="false">IF($D12="","",IF(AND(TIMEVALUE(N$1)&gt;=TIMEVALUE($D12),TIMEVALUE(N$1)&lt;TIMEVALUE($E12)),1,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11" t="str">
+        <f aca="false">IF($B13&lt;&gt;"",AND($D13&lt;&gt;"",$E13&lt;&gt;""),"")</f>
+        <v/>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="10" t="str">
+        <f aca="false">IF($D13="","",IF(AND(TIMEVALUE(F$1)&gt;=TIMEVALUE($D13),TIMEVALUE(F$1)&lt;TIMEVALUE($E13)),1,""))</f>
+        <v/>
+      </c>
+      <c r="G13" s="10" t="str">
+        <f aca="false">IF($D13="","",IF(AND(TIMEVALUE(G$1)&gt;=TIMEVALUE($D13),TIMEVALUE(G$1)&lt;TIMEVALUE($E13)),1,""))</f>
+        <v/>
+      </c>
+      <c r="H13" s="10" t="str">
+        <f aca="false">IF($D13="","",IF(AND(TIMEVALUE(H$1)&gt;=TIMEVALUE($D13),TIMEVALUE(H$1)&lt;TIMEVALUE($E13)),1,""))</f>
+        <v/>
+      </c>
+      <c r="I13" s="10" t="str">
+        <f aca="false">IF($D13="","",IF(AND(TIMEVALUE(I$1)&gt;=TIMEVALUE($D13),TIMEVALUE(I$1)&lt;TIMEVALUE($E13)),1,""))</f>
+        <v/>
+      </c>
+      <c r="J13" s="10" t="str">
+        <f aca="false">IF($D13="","",IF(AND(TIMEVALUE(J$1)&gt;=TIMEVALUE($D13),TIMEVALUE(J$1)&lt;TIMEVALUE($E13)),1,""))</f>
+        <v/>
+      </c>
+      <c r="K13" s="10" t="str">
+        <f aca="false">IF($D13="","",IF(AND(TIMEVALUE(K$1)&gt;=TIMEVALUE($D13),TIMEVALUE(K$1)&lt;TIMEVALUE($E13)),1,""))</f>
+        <v/>
+      </c>
+      <c r="L13" s="10" t="str">
+        <f aca="false">IF($D13="","",IF(AND(TIMEVALUE(L$1)&gt;=TIMEVALUE($D13),TIMEVALUE(L$1)&lt;TIMEVALUE($E13)),1,""))</f>
+        <v/>
+      </c>
+      <c r="M13" s="10" t="str">
+        <f aca="false">IF($D13="","",IF(AND(TIMEVALUE(M$1)&gt;=TIMEVALUE($D13),TIMEVALUE(M$1)&lt;TIMEVALUE($E13)),1,""))</f>
+        <v/>
+      </c>
+      <c r="N13" s="10" t="str">
+        <f aca="false">IF($D13="","",IF(AND(TIMEVALUE(N$1)&gt;=TIMEVALUE($D13),TIMEVALUE(N$1)&lt;TIMEVALUE($E13)),1,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11" t="str">
+        <f aca="false">IF($B14&lt;&gt;"",AND($D14&lt;&gt;"",$E14&lt;&gt;""),"")</f>
+        <v/>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="10" t="str">
+        <f aca="false">IF($D14="","",IF(AND(TIMEVALUE(F$1)&gt;=TIMEVALUE($D14),TIMEVALUE(F$1)&lt;TIMEVALUE($E14)),1,""))</f>
+        <v/>
+      </c>
+      <c r="G14" s="10" t="str">
+        <f aca="false">IF($D14="","",IF(AND(TIMEVALUE(G$1)&gt;=TIMEVALUE($D14),TIMEVALUE(G$1)&lt;TIMEVALUE($E14)),1,""))</f>
+        <v/>
+      </c>
+      <c r="H14" s="10" t="str">
+        <f aca="false">IF($D14="","",IF(AND(TIMEVALUE(H$1)&gt;=TIMEVALUE($D14),TIMEVALUE(H$1)&lt;TIMEVALUE($E14)),1,""))</f>
+        <v/>
+      </c>
+      <c r="I14" s="10" t="str">
+        <f aca="false">IF($D14="","",IF(AND(TIMEVALUE(I$1)&gt;=TIMEVALUE($D14),TIMEVALUE(I$1)&lt;TIMEVALUE($E14)),1,""))</f>
+        <v/>
+      </c>
+      <c r="J14" s="10" t="str">
+        <f aca="false">IF($D14="","",IF(AND(TIMEVALUE(J$1)&gt;=TIMEVALUE($D14),TIMEVALUE(J$1)&lt;TIMEVALUE($E14)),1,""))</f>
+        <v/>
+      </c>
+      <c r="K14" s="10" t="str">
+        <f aca="false">IF($D14="","",IF(AND(TIMEVALUE(K$1)&gt;=TIMEVALUE($D14),TIMEVALUE(K$1)&lt;TIMEVALUE($E14)),1,""))</f>
+        <v/>
+      </c>
+      <c r="L14" s="10" t="str">
+        <f aca="false">IF($D14="","",IF(AND(TIMEVALUE(L$1)&gt;=TIMEVALUE($D14),TIMEVALUE(L$1)&lt;TIMEVALUE($E14)),1,""))</f>
+        <v/>
+      </c>
+      <c r="M14" s="10" t="str">
+        <f aca="false">IF($D14="","",IF(AND(TIMEVALUE(M$1)&gt;=TIMEVALUE($D14),TIMEVALUE(M$1)&lt;TIMEVALUE($E14)),1,""))</f>
+        <v/>
+      </c>
+      <c r="N14" s="10" t="str">
+        <f aca="false">IF($D14="","",IF(AND(TIMEVALUE(N$1)&gt;=TIMEVALUE($D14),TIMEVALUE(N$1)&lt;TIMEVALUE($E14)),1,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11" t="str">
+        <f aca="false">IF($B15&lt;&gt;"",AND($D15&lt;&gt;"",$E15&lt;&gt;""),"")</f>
+        <v/>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="10" t="str">
+        <f aca="false">IF($D15="","",IF(AND(TIMEVALUE(F$1)&gt;=TIMEVALUE($D15),TIMEVALUE(F$1)&lt;TIMEVALUE($E15)),1,""))</f>
+        <v/>
+      </c>
+      <c r="G15" s="10" t="str">
+        <f aca="false">IF($D15="","",IF(AND(TIMEVALUE(G$1)&gt;=TIMEVALUE($D15),TIMEVALUE(G$1)&lt;TIMEVALUE($E15)),1,""))</f>
+        <v/>
+      </c>
+      <c r="H15" s="10" t="str">
+        <f aca="false">IF($D15="","",IF(AND(TIMEVALUE(H$1)&gt;=TIMEVALUE($D15),TIMEVALUE(H$1)&lt;TIMEVALUE($E15)),1,""))</f>
+        <v/>
+      </c>
+      <c r="I15" s="10" t="str">
+        <f aca="false">IF($D15="","",IF(AND(TIMEVALUE(I$1)&gt;=TIMEVALUE($D15),TIMEVALUE(I$1)&lt;TIMEVALUE($E15)),1,""))</f>
+        <v/>
+      </c>
+      <c r="J15" s="10" t="str">
+        <f aca="false">IF($D15="","",IF(AND(TIMEVALUE(J$1)&gt;=TIMEVALUE($D15),TIMEVALUE(J$1)&lt;TIMEVALUE($E15)),1,""))</f>
+        <v/>
+      </c>
+      <c r="K15" s="10" t="str">
+        <f aca="false">IF($D15="","",IF(AND(TIMEVALUE(K$1)&gt;=TIMEVALUE($D15),TIMEVALUE(K$1)&lt;TIMEVALUE($E15)),1,""))</f>
+        <v/>
+      </c>
+      <c r="L15" s="10" t="str">
+        <f aca="false">IF($D15="","",IF(AND(TIMEVALUE(L$1)&gt;=TIMEVALUE($D15),TIMEVALUE(L$1)&lt;TIMEVALUE($E15)),1,""))</f>
+        <v/>
+      </c>
+      <c r="M15" s="10" t="str">
+        <f aca="false">IF($D15="","",IF(AND(TIMEVALUE(M$1)&gt;=TIMEVALUE($D15),TIMEVALUE(M$1)&lt;TIMEVALUE($E15)),1,""))</f>
+        <v/>
+      </c>
+      <c r="N15" s="10" t="str">
+        <f aca="false">IF($D15="","",IF(AND(TIMEVALUE(N$1)&gt;=TIMEVALUE($D15),TIMEVALUE(N$1)&lt;TIMEVALUE($E15)),1,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11" t="str">
+        <f aca="false">IF($B16&lt;&gt;"",AND($D16&lt;&gt;"",$E16&lt;&gt;""),"")</f>
+        <v/>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="10" t="str">
+        <f aca="false">IF($D16="","",IF(AND(TIMEVALUE(F$1)&gt;=TIMEVALUE($D16),TIMEVALUE(F$1)&lt;TIMEVALUE($E16)),1,""))</f>
+        <v/>
+      </c>
+      <c r="G16" s="10" t="str">
+        <f aca="false">IF($D16="","",IF(AND(TIMEVALUE(G$1)&gt;=TIMEVALUE($D16),TIMEVALUE(G$1)&lt;TIMEVALUE($E16)),1,""))</f>
+        <v/>
+      </c>
+      <c r="H16" s="10" t="str">
+        <f aca="false">IF($D16="","",IF(AND(TIMEVALUE(H$1)&gt;=TIMEVALUE($D16),TIMEVALUE(H$1)&lt;TIMEVALUE($E16)),1,""))</f>
+        <v/>
+      </c>
+      <c r="I16" s="10" t="str">
+        <f aca="false">IF($D16="","",IF(AND(TIMEVALUE(I$1)&gt;=TIMEVALUE($D16),TIMEVALUE(I$1)&lt;TIMEVALUE($E16)),1,""))</f>
+        <v/>
+      </c>
+      <c r="J16" s="10" t="str">
+        <f aca="false">IF($D16="","",IF(AND(TIMEVALUE(J$1)&gt;=TIMEVALUE($D16),TIMEVALUE(J$1)&lt;TIMEVALUE($E16)),1,""))</f>
+        <v/>
+      </c>
+      <c r="K16" s="10" t="str">
+        <f aca="false">IF($D16="","",IF(AND(TIMEVALUE(K$1)&gt;=TIMEVALUE($D16),TIMEVALUE(K$1)&lt;TIMEVALUE($E16)),1,""))</f>
+        <v/>
+      </c>
+      <c r="L16" s="10" t="str">
+        <f aca="false">IF($D16="","",IF(AND(TIMEVALUE(L$1)&gt;=TIMEVALUE($D16),TIMEVALUE(L$1)&lt;TIMEVALUE($E16)),1,""))</f>
+        <v/>
+      </c>
+      <c r="M16" s="10" t="str">
+        <f aca="false">IF($D16="","",IF(AND(TIMEVALUE(M$1)&gt;=TIMEVALUE($D16),TIMEVALUE(M$1)&lt;TIMEVALUE($E16)),1,""))</f>
+        <v/>
+      </c>
+      <c r="N16" s="10" t="str">
+        <f aca="false">IF($D16="","",IF(AND(TIMEVALUE(N$1)&gt;=TIMEVALUE($D16),TIMEVALUE(N$1)&lt;TIMEVALUE($E16)),1,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11" t="str">
+        <f aca="false">IF($B17&lt;&gt;"",AND($D17&lt;&gt;"",$E17&lt;&gt;""),"")</f>
+        <v/>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="10" t="str">
+        <f aca="false">IF($D17="","",IF(AND(TIMEVALUE(F$1)&gt;=TIMEVALUE($D17),TIMEVALUE(F$1)&lt;TIMEVALUE($E17)),1,""))</f>
+        <v/>
+      </c>
+      <c r="G17" s="10" t="str">
+        <f aca="false">IF($D17="","",IF(AND(TIMEVALUE(G$1)&gt;=TIMEVALUE($D17),TIMEVALUE(G$1)&lt;TIMEVALUE($E17)),1,""))</f>
+        <v/>
+      </c>
+      <c r="H17" s="10" t="str">
+        <f aca="false">IF($D17="","",IF(AND(TIMEVALUE(H$1)&gt;=TIMEVALUE($D17),TIMEVALUE(H$1)&lt;TIMEVALUE($E17)),1,""))</f>
+        <v/>
+      </c>
+      <c r="I17" s="10" t="str">
+        <f aca="false">IF($D17="","",IF(AND(TIMEVALUE(I$1)&gt;=TIMEVALUE($D17),TIMEVALUE(I$1)&lt;TIMEVALUE($E17)),1,""))</f>
+        <v/>
+      </c>
+      <c r="J17" s="10" t="str">
+        <f aca="false">IF($D17="","",IF(AND(TIMEVALUE(J$1)&gt;=TIMEVALUE($D17),TIMEVALUE(J$1)&lt;TIMEVALUE($E17)),1,""))</f>
+        <v/>
+      </c>
+      <c r="K17" s="10" t="str">
+        <f aca="false">IF($D17="","",IF(AND(TIMEVALUE(K$1)&gt;=TIMEVALUE($D17),TIMEVALUE(K$1)&lt;TIMEVALUE($E17)),1,""))</f>
+        <v/>
+      </c>
+      <c r="L17" s="10" t="str">
+        <f aca="false">IF($D17="","",IF(AND(TIMEVALUE(L$1)&gt;=TIMEVALUE($D17),TIMEVALUE(L$1)&lt;TIMEVALUE($E17)),1,""))</f>
+        <v/>
+      </c>
+      <c r="M17" s="10" t="str">
+        <f aca="false">IF($D17="","",IF(AND(TIMEVALUE(M$1)&gt;=TIMEVALUE($D17),TIMEVALUE(M$1)&lt;TIMEVALUE($E17)),1,""))</f>
+        <v/>
+      </c>
+      <c r="N17" s="10" t="str">
+        <f aca="false">IF($D17="","",IF(AND(TIMEVALUE(N$1)&gt;=TIMEVALUE($D17),TIMEVALUE(N$1)&lt;TIMEVALUE($E17)),1,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="11" t="str">
+        <f aca="false">IF($B18&lt;&gt;"",AND($D18&lt;&gt;"",$E18&lt;&gt;""),"")</f>
+        <v/>
+      </c>
+      <c r="D18" s="15"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="10" t="str">
+        <f aca="false">IF($D18="","",IF(AND(TIMEVALUE(F$1)&gt;=TIMEVALUE($D18),TIMEVALUE(F$1)&lt;TIMEVALUE($E18)),1,""))</f>
+        <v/>
+      </c>
+      <c r="G18" s="10" t="str">
+        <f aca="false">IF($D18="","",IF(AND(TIMEVALUE(G$1)&gt;=TIMEVALUE($D18),TIMEVALUE(G$1)&lt;TIMEVALUE($E18)),1,""))</f>
+        <v/>
+      </c>
+      <c r="H18" s="10" t="str">
+        <f aca="false">IF($D18="","",IF(AND(TIMEVALUE(H$1)&gt;=TIMEVALUE($D18),TIMEVALUE(H$1)&lt;TIMEVALUE($E18)),1,""))</f>
+        <v/>
+      </c>
+      <c r="I18" s="10" t="str">
+        <f aca="false">IF($D18="","",IF(AND(TIMEVALUE(I$1)&gt;=TIMEVALUE($D18),TIMEVALUE(I$1)&lt;TIMEVALUE($E18)),1,""))</f>
+        <v/>
+      </c>
+      <c r="J18" s="10" t="str">
+        <f aca="false">IF($D18="","",IF(AND(TIMEVALUE(J$1)&gt;=TIMEVALUE($D18),TIMEVALUE(J$1)&lt;TIMEVALUE($E18)),1,""))</f>
+        <v/>
+      </c>
+      <c r="K18" s="10" t="str">
+        <f aca="false">IF($D18="","",IF(AND(TIMEVALUE(K$1)&gt;=TIMEVALUE($D18),TIMEVALUE(K$1)&lt;TIMEVALUE($E18)),1,""))</f>
+        <v/>
+      </c>
+      <c r="L18" s="10" t="str">
+        <f aca="false">IF($D18="","",IF(AND(TIMEVALUE(L$1)&gt;=TIMEVALUE($D18),TIMEVALUE(L$1)&lt;TIMEVALUE($E18)),1,""))</f>
+        <v/>
+      </c>
+      <c r="M18" s="10" t="str">
+        <f aca="false">IF($D18="","",IF(AND(TIMEVALUE(M$1)&gt;=TIMEVALUE($D18),TIMEVALUE(M$1)&lt;TIMEVALUE($E18)),1,""))</f>
+        <v/>
+      </c>
+      <c r="N18" s="10" t="str">
+        <f aca="false">IF($D18="","",IF(AND(TIMEVALUE(N$1)&gt;=TIMEVALUE($D18),TIMEVALUE(N$1)&lt;TIMEVALUE($E18)),1,""))</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="F2:N18">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,標準"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,標準"&amp;12ページ &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>